<commit_message>
Start date changed to August 30
</commit_message>
<xml_diff>
--- a/Index Portfolio.xlsx
+++ b/Index Portfolio.xlsx
@@ -8,13 +8,34 @@
   </bookViews>
   <sheets>
     <sheet name="portfolio.data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="portfolio.data" localSheetId="1">Sheet1!$A$1:$F$26</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="portfolio.data" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Alexander\test\portanalysis-indexportfolio\portfolio.data.csv" comma="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>Share</t>
   </si>
@@ -654,6 +675,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="portfolio.data" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1491,4 +1516,544 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>72.84</v>
+      </c>
+      <c r="D2">
+        <v>99869</v>
+      </c>
+      <c r="E2" s="1">
+        <v>7274457.96</v>
+      </c>
+      <c r="F2" s="2">
+        <v>7.2744760255628704E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>35.75</v>
+      </c>
+      <c r="D3">
+        <v>420378</v>
+      </c>
+      <c r="E3" s="1">
+        <v>15028513.5</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.150285217017984</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>31.39</v>
+      </c>
+      <c r="D4">
+        <v>209013</v>
+      </c>
+      <c r="E4" s="1">
+        <v>6560918.0700000003</v>
+      </c>
+      <c r="F4" s="2">
+        <v>6.5609486215004204E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>29.69</v>
+      </c>
+      <c r="D5">
+        <v>161904</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4806929.76</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4.8069522516317402E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1">
+        <v>32.450000000000003</v>
+      </c>
+      <c r="D6">
+        <v>178705</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5798977.25</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5.79899513350269E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D7">
+        <v>1260412</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6176018.7999999998</v>
+      </c>
+      <c r="F7" s="2">
+        <v>6.1760208997869097E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1">
+        <v>35.67</v>
+      </c>
+      <c r="D8">
+        <v>125740</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4485145.8</v>
+      </c>
+      <c r="F8" s="2">
+        <v>4.4851492531327003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1">
+        <v>40.659999999999997</v>
+      </c>
+      <c r="D9">
+        <v>95163</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3869327.58</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3.8693681761386697E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1">
+        <v>67.989999999999995</v>
+      </c>
+      <c r="D10">
+        <v>47462</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3226941.38</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3.2269998150353599E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1">
+        <v>38.18</v>
+      </c>
+      <c r="D11">
+        <v>98692</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3768060.56</v>
+      </c>
+      <c r="F11" s="2">
+        <v>3.7680742983483097E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1">
+        <v>58.3</v>
+      </c>
+      <c r="D12">
+        <v>61522</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3586732.6</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3.5867844482978098E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1">
+        <v>11.08</v>
+      </c>
+      <c r="D13">
+        <v>313086</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3468992.88</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3.4689986330970403E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1">
+        <v>15.2</v>
+      </c>
+      <c r="D14">
+        <v>181925</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2765260</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2.7652643856862301E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1">
+        <v>43.86</v>
+      </c>
+      <c r="D15">
+        <v>49902</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2188701.7200000002</v>
+      </c>
+      <c r="F15" s="2">
+        <v>2.1887369329039501E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1">
+        <v>13.25</v>
+      </c>
+      <c r="D16">
+        <v>271200</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3593400</v>
+      </c>
+      <c r="F16" s="2">
+        <v>3.5934052278667097E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4.74</v>
+      </c>
+      <c r="D17">
+        <v>656315</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3110933.1</v>
+      </c>
+      <c r="F17" s="2">
+        <v>3.1109344850409001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="D18">
+        <v>255483</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2146057.2000000002</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2.1460622055074801E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1">
+        <v>14.61</v>
+      </c>
+      <c r="D19">
+        <v>159783</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2334429.63</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2.3344354971038699E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="1">
+        <v>13.26</v>
+      </c>
+      <c r="D20">
+        <v>182691</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2422482.66</v>
+      </c>
+      <c r="F20" s="2">
+        <v>2.4224838197648899E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3.73</v>
+      </c>
+      <c r="D21">
+        <v>571406</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2131344.38</v>
+      </c>
+      <c r="F21" s="2">
+        <v>2.1313448453821299E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1">
+        <v>15.75</v>
+      </c>
+      <c r="D22">
+        <v>157464</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2480058</v>
+      </c>
+      <c r="F22" s="2">
+        <v>2.48006268248489E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="1">
+        <v>35.450000000000003</v>
+      </c>
+      <c r="D23">
+        <v>62124</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2202295.7999999998</v>
+      </c>
+      <c r="F23" s="2">
+        <v>2.2023055046148599E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2.59</v>
+      </c>
+      <c r="D24">
+        <v>835506</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2163960.54</v>
+      </c>
+      <c r="F24" s="2">
+        <v>2.1639615483585201E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="1">
+        <v>5.46</v>
+      </c>
+      <c r="D25">
+        <v>400115</v>
+      </c>
+      <c r="E25" s="1">
+        <v>2184627.9</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2.1846282579790599E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="D26">
+        <v>684641</v>
+      </c>
+      <c r="E26" s="1">
+        <v>2225083.25</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2.2250853494736E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>